<commit_message>
Added bar chart to jupyter notebook.
</commit_message>
<xml_diff>
--- a/Homework.xlsx
+++ b/Homework.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B39D4D-AD10-484B-8460-F3EA75193115}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD8DB54-A085-490A-A738-63ACB5537BD9}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Spring" sheetId="2" r:id="rId1"/>
@@ -978,7 +978,7 @@
                   <c:v>34.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>72.5</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>18</c:v>
@@ -1762,7 +1762,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Author" refreshedDate="43194.06431898148" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="47" xr:uid="{278637BA-FCB9-4CF2-83CE-0EDCAA1E69F6}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Author" refreshedDate="43194.879973379633" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="47" xr:uid="{278637BA-FCB9-4CF2-83CE-0EDCAA1E69F6}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:I48" sheet="Spring"/>
   </cacheSource>
@@ -2252,7 +2252,7 @@
     <s v="HW1"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="Not that bad actually"/>
+    <s v="Not bad"/>
     <n v="7"/>
     <n v="0.84"/>
     <m/>
@@ -2263,7 +2263,7 @@
     <s v="Homework 1"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="Hard af"/>
+    <s v="Hard"/>
     <n v="7"/>
     <n v="0.7"/>
     <m/>
@@ -2274,7 +2274,7 @@
     <s v="HW2"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="Not bad at all"/>
+    <s v="Not bad"/>
     <n v="3"/>
     <n v="1.1599999999999999"/>
     <m/>
@@ -2285,7 +2285,7 @@
     <s v="Homework 1"/>
     <s v="Skipped"/>
     <n v="0"/>
-    <s v="Lengthy but not 121 hard"/>
+    <s v="Lengthy"/>
     <n v="1"/>
     <n v="0"/>
     <m/>
@@ -2296,7 +2296,7 @@
     <s v="Homework 2"/>
     <s v="Skipped"/>
     <n v="0"/>
-    <s v="Hard af"/>
+    <s v="Hard"/>
     <n v="0"/>
     <n v="0"/>
     <m/>
@@ -2307,7 +2307,7 @@
     <s v="HW3"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="Guessing won't be hard"/>
+    <s v="Not bad"/>
     <n v="8"/>
     <n v="0.84"/>
     <m/>
@@ -2318,7 +2318,7 @@
     <s v="Homework 2"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="Doesn't look hard"/>
+    <s v="Easy"/>
     <n v="3"/>
     <m/>
     <m/>
@@ -2340,7 +2340,7 @@
     <s v="Midterm 1 (in class)"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="We'll see"/>
+    <s v="Not sure"/>
     <n v="1.5"/>
     <n v="0.78"/>
     <n v="0.88"/>
@@ -2362,7 +2362,7 @@
     <s v="User Stories"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="idk"/>
+    <s v="Not sure"/>
     <n v="2"/>
     <n v="1"/>
     <m/>
@@ -2373,7 +2373,7 @@
     <s v="Homework 3"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="Not quite so bad"/>
+    <s v="Not bad"/>
     <n v="3"/>
     <n v="0.65"/>
     <m/>
@@ -2384,7 +2384,7 @@
     <s v="Midterm 1 (tentative)"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="RIP"/>
+    <s v="Heinous garbage"/>
     <n v="7.5"/>
     <n v="0.86"/>
     <n v="0.85"/>
@@ -2395,7 +2395,7 @@
     <s v="Homework 2"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="We'll see"/>
+    <s v="Not sure"/>
     <n v="4"/>
     <m/>
     <m/>
@@ -2406,7 +2406,7 @@
     <s v="HW5"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="Not as bad now"/>
+    <s v="Not bad"/>
     <n v="5.5"/>
     <n v="0.95"/>
     <m/>
@@ -2417,7 +2417,7 @@
     <s v="Homework 2 Part 2"/>
     <s v="Gave Up"/>
     <n v="0"/>
-    <s v="Probably hard"/>
+    <s v="Hard"/>
     <n v="14.5"/>
     <m/>
     <m/>
@@ -2428,7 +2428,7 @@
     <s v="HW6"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="Easier than anticipated"/>
+    <s v="Easy"/>
     <n v="6.25"/>
     <n v="1"/>
     <m/>
@@ -2450,7 +2450,7 @@
     <s v="First Iteration"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="Need to practice Django"/>
+    <s v="Hard"/>
     <n v="12.5"/>
     <n v="1"/>
     <m/>
@@ -2461,7 +2461,7 @@
     <s v="Homework 3"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="More Android; no late days"/>
+    <s v="A bit tough"/>
     <n v="4"/>
     <m/>
     <m/>
@@ -2472,7 +2472,7 @@
     <s v="Homework 3"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="Depends"/>
+    <s v="Not sure"/>
     <n v="3"/>
     <m/>
     <m/>
@@ -2483,7 +2483,7 @@
     <s v="HW7"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="Hopefully not awful"/>
+    <s v="Not bad"/>
     <n v="8.5"/>
     <m/>
     <m/>
@@ -2494,7 +2494,7 @@
     <s v="Midterm"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="Don't know"/>
+    <s v="Not sure"/>
     <n v="1.5"/>
     <m/>
     <m/>
@@ -2505,7 +2505,7 @@
     <s v="Homework 5"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="More heinous garbage"/>
+    <s v="Heinous garbage"/>
     <n v="4"/>
     <m/>
     <m/>
@@ -2516,7 +2516,7 @@
     <s v="Project Proposal"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="Probably not too bad"/>
+    <s v="Not bad"/>
     <n v="1"/>
     <m/>
     <m/>
@@ -2527,7 +2527,7 @@
     <s v="Homework 4"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="Depends"/>
+    <s v="Not bad"/>
     <n v="4"/>
     <m/>
     <m/>
@@ -2538,7 +2538,7 @@
     <s v="Homework 4: Part 1"/>
     <s v="Skipped"/>
     <n v="0"/>
-    <s v="Easy I think"/>
+    <s v="Easy"/>
     <n v="0"/>
     <m/>
     <m/>
@@ -2549,7 +2549,7 @@
     <s v="Midterm (tentative)"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="We'll see"/>
+    <s v="Not sure"/>
     <n v="5"/>
     <m/>
     <m/>
@@ -2560,7 +2560,7 @@
     <s v="Update Meeting"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="Just an update meeting"/>
+    <s v="Easy"/>
     <n v="2"/>
     <m/>
     <m/>
@@ -2571,7 +2571,7 @@
     <s v="Group Update Meeting"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="Need to have some stuff"/>
+    <s v="A bit tough"/>
     <n v="4"/>
     <m/>
     <m/>
@@ -2582,7 +2582,7 @@
     <s v="HW8"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="Not that bad!"/>
+    <s v="Not bad"/>
     <n v="6"/>
     <m/>
     <m/>
@@ -2593,7 +2593,7 @@
     <s v="Midterm (tentative)"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="Not sure at all"/>
+    <s v="Not sure"/>
     <n v="3"/>
     <m/>
     <m/>
@@ -2604,7 +2604,7 @@
     <s v="Homework 6"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="Maybe not impossible"/>
+    <s v="Not bad"/>
     <n v="4"/>
     <m/>
     <m/>
@@ -2615,7 +2615,7 @@
     <s v="Group Update Meeting"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="Just need to refactor &amp; test"/>
+    <s v="Easy"/>
     <n v="11.5"/>
     <m/>
     <m/>
@@ -2626,7 +2626,7 @@
     <s v="Midterm 2 (tentative)"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="P O S T P O N E D"/>
+    <s v="Not sure"/>
     <n v="4"/>
     <m/>
     <m/>
@@ -2637,7 +2637,7 @@
     <s v="Midterm 2 (tentative)"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="Better hope not"/>
+    <s v="Hard"/>
     <n v="7"/>
     <m/>
     <m/>
@@ -2648,7 +2648,7 @@
     <s v="Homework 4"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="Might be tough, ~7 hours?"/>
+    <s v="Lengthy"/>
     <n v="15"/>
     <m/>
     <m/>
@@ -2659,7 +2659,7 @@
     <s v="HW9"/>
     <s v="Completed"/>
     <n v="0"/>
-    <s v="Might need help"/>
+    <s v="A bit tough"/>
     <n v="5"/>
     <m/>
     <m/>
@@ -2668,10 +2668,10 @@
     <x v="2"/>
     <x v="26"/>
     <s v="Group Update Meeting"/>
-    <s v="In Progress"/>
+    <s v="Completed"/>
     <n v="0"/>
-    <s v="maybe 5ish hours?"/>
-    <n v="0.5"/>
+    <s v="A bit tough"/>
+    <n v="3"/>
     <m/>
     <m/>
   </r>
@@ -2681,7 +2681,7 @@
     <s v="HW10"/>
     <s v="In Progress"/>
     <n v="1"/>
-    <s v="Almost done"/>
+    <s v="A bit tough"/>
     <n v="4"/>
     <m/>
     <m/>
@@ -2692,7 +2692,7 @@
     <s v="Iteration 3 Meeting"/>
     <s v="Haven't Started"/>
     <n v="2"/>
-    <s v="vote sorting, related q, hyperlink"/>
+    <s v="A bit tough"/>
     <m/>
     <m/>
     <m/>
@@ -2703,7 +2703,7 @@
     <s v="Homework 7"/>
     <s v="Haven't Started"/>
     <n v="8"/>
-    <s v="he might add additional problems"/>
+    <s v="Hard"/>
     <m/>
     <m/>
     <m/>
@@ -2714,7 +2714,7 @@
     <s v="Homework 5"/>
     <s v="In Progress"/>
     <n v="9"/>
-    <s v="Probably another 15 hours or so"/>
+    <s v="Lengthy"/>
     <n v="1"/>
     <m/>
     <m/>
@@ -3554,8 +3554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C7F483A-6388-4F0D-80E8-A83342E604EB}">
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView topLeftCell="A32" zoomScale="109" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3565,7 +3565,7 @@
     <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
@@ -3635,7 +3635,7 @@
       <c r="I2" s="29"/>
       <c r="K2" s="47">
         <f>SUM(G2:G125)</f>
-        <v>200</v>
+        <v>202.5</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -4663,30 +4663,30 @@
       <c r="I39" s="29"/>
     </row>
     <row r="40" spans="1:9" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="62" t="s">
+      <c r="A40" s="54" t="s">
         <v>151</v>
       </c>
-      <c r="B40" s="36">
+      <c r="B40" s="30">
         <v>43194</v>
       </c>
-      <c r="C40" s="32" t="s">
+      <c r="C40" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="D40" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="E40" s="63">
+      <c r="D40" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" s="31">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="F40" s="32" t="s">
+      <c r="F40" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="G40" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="H40" s="32"/>
-      <c r="I40" s="32"/>
+      <c r="G40" s="29">
+        <v>3</v>
+      </c>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
     </row>
     <row r="41" spans="1:9" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="62" t="s">
@@ -4879,8 +4879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B0251A0-FC32-431A-9EE7-B5456C2DA0CD}">
   <dimension ref="A3:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4918,7 +4918,7 @@
         <v>151</v>
       </c>
       <c r="B6" s="52">
-        <v>72.5</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -4943,7 +4943,7 @@
       </c>
       <c r="B10">
         <f>SUM(B4:B8)</f>
-        <v>200</v>
+        <v>202.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>